<commit_message>
SeparateData: added alternative self-report analysis, added plots  PlotResults: plot offer as function of emotion strength
Signed-off-by: Chaviva Moshavi <chaviva.moshavi@gmail.com>
</commit_message>
<xml_diff>
--- a/data/AudioBaseline.xlsx
+++ b/data/AudioBaseline.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B5C881-180C-46E2-8901-D4E536EA1274}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B5C3929-9CB5-4779-AC52-1FF4AF2F3609}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="6">
   <si>
     <t>Neutral</t>
   </si>
@@ -358,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D156"/>
+  <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D156"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="J176" sqref="J176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2537,16 +2537,366 @@
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A156" s="1" t="s">
+      <c r="A156" s="1">
+        <v>156</v>
+      </c>
+      <c r="B156" s="1">
+        <v>1032</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D156" s="1">
+        <v>0.18229999999999999</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157" s="1">
+        <v>157</v>
+      </c>
+      <c r="B157" s="1">
+        <v>1032</v>
+      </c>
+      <c r="C157" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D157" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158" s="1">
+        <v>158</v>
+      </c>
+      <c r="B158" s="1">
+        <v>1032</v>
+      </c>
+      <c r="C158" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D158" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159" s="1">
+        <v>159</v>
+      </c>
+      <c r="B159" s="1">
+        <v>1032</v>
+      </c>
+      <c r="C159" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D159" s="1">
+        <v>1.34E-2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160" s="1">
+        <v>160</v>
+      </c>
+      <c r="B160" s="1">
+        <v>1032</v>
+      </c>
+      <c r="C160" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D160" s="1">
+        <v>0.80410000000000004</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161" s="1">
+        <v>161</v>
+      </c>
+      <c r="B161" s="1">
+        <v>1033</v>
+      </c>
+      <c r="C161" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D161" s="1">
+        <v>0.1769</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162" s="1">
+        <v>162</v>
+      </c>
+      <c r="B162" s="1">
+        <v>1033</v>
+      </c>
+      <c r="C162" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D162" s="1">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163" s="1">
+        <v>163</v>
+      </c>
+      <c r="B163" s="1">
+        <v>1033</v>
+      </c>
+      <c r="C163" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D163" s="1">
+        <v>0.79210000000000003</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164" s="1">
+        <v>164</v>
+      </c>
+      <c r="B164" s="1">
+        <v>1033</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D164" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165" s="1">
+        <v>165</v>
+      </c>
+      <c r="B165" s="1">
+        <v>1033</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D165" s="1">
+        <v>3.0200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166" s="1">
+        <v>166</v>
+      </c>
+      <c r="B166" s="1">
+        <v>1035</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D166" s="1">
+        <v>0.21529999999999999</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167" s="1">
+        <v>167</v>
+      </c>
+      <c r="B167" s="1">
+        <v>1035</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D167" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168" s="1">
+        <v>168</v>
+      </c>
+      <c r="B168" s="1">
+        <v>1035</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D168" s="1">
+        <v>0.77569999999999995</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169" s="1">
+        <v>169</v>
+      </c>
+      <c r="B169" s="1">
+        <v>1035</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D169" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170" s="1">
+        <v>170</v>
+      </c>
+      <c r="B170" s="1">
+        <v>1035</v>
+      </c>
+      <c r="C170" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D170" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171" s="1">
+        <v>171</v>
+      </c>
+      <c r="B171" s="1">
+        <v>1039</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D171" s="1">
+        <v>0.94199999999999995</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172" s="1">
+        <v>172</v>
+      </c>
+      <c r="B172" s="1">
+        <v>1039</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D172" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173" s="1">
+        <v>173</v>
+      </c>
+      <c r="B173" s="1">
+        <v>1039</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D173" s="1">
+        <v>5.1200000000000002E-2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174" s="1">
+        <v>174</v>
+      </c>
+      <c r="B174" s="1">
+        <v>1039</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D174" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175" s="1">
+        <v>175</v>
+      </c>
+      <c r="B175" s="1">
+        <v>1039</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D175" s="1">
+        <v>6.8999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176" s="1">
+        <v>176</v>
+      </c>
+      <c r="B176" s="1">
+        <v>1038</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D176" s="1">
+        <v>2.41E-2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177" s="1">
+        <v>177</v>
+      </c>
+      <c r="B177" s="1">
+        <v>1038</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D177" s="1">
+        <v>1.6299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178" s="1">
+        <v>178</v>
+      </c>
+      <c r="B178" s="1">
+        <v>1038</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D178" s="1">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179" s="1">
+        <v>179</v>
+      </c>
+      <c r="B179" s="1">
+        <v>1038</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D179" s="1">
+        <v>4.8500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180" s="1">
+        <v>180</v>
+      </c>
+      <c r="B180" s="1">
+        <v>1038</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D180" s="1">
+        <v>0.90969999999999995</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B156" s="1" t="s">
+      <c r="B181" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C156" s="1" t="s">
+      <c r="C181" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D156" s="1" t="s">
+      <c r="D181" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>